<commit_message>
update with trendlines and borders
</commit_message>
<xml_diff>
--- a/George-Yanev-Milwaukee-Popov.xlsx
+++ b/George-Yanev-Milwaukee-Popov.xlsx
@@ -287,6 +287,7 @@
     <font>
       <name val="Arial"/>
       <family val="2"/>
+      <b val="true"/>
       <sz val="13"/>
     </font>
     <font>
@@ -513,7 +514,7 @@
 </styleSheet>
 </file>
 
-<file path=xl/charts/chart389.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/charts/chart109.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:lang val="en-US"/>
   <c:chart>
@@ -528,7 +529,7 @@
               <a:defRPr/>
             </a:pPr>
             <a:r>
-              <a:rPr sz="1300"/>
+              <a:rPr b="1" sz="1300"/>
               <a:t>Milwaukee Airport Средни месечни температури за 2та периода</a:t>
             </a:r>
           </a:p>
@@ -776,11 +777,11 @@
           </c:val>
         </c:ser>
         <c:marker val="0"/>
-        <c:axId val="34729009"/>
-        <c:axId val="40784176"/>
+        <c:axId val="60584489"/>
+        <c:axId val="79094754"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="34729009"/>
+        <c:axId val="60584489"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -796,14 +797,14 @@
             </a:solidFill>
           </a:ln>
         </c:spPr>
-        <c:crossAx val="40784176"/>
+        <c:crossAx val="79094754"/>
         <c:crossesAt val="0"/>
         <c:lblAlgn val="ctr"/>
         <c:auto val="1"/>
         <c:lblOffset val="100"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="40784176"/>
+        <c:axId val="79094754"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -828,7 +829,7 @@
             </a:solidFill>
           </a:ln>
         </c:spPr>
-        <c:crossAx val="34729009"/>
+        <c:crossAx val="60584489"/>
         <c:crossesAt val="0"/>
       </c:valAx>
       <c:spPr>
@@ -856,7 +857,7 @@
 </c:chartSpace>
 </file>
 
-<file path=xl/charts/chart390.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/charts/chart110.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:lang val="en-US"/>
   <c:chart>
@@ -871,7 +872,7 @@
               <a:defRPr/>
             </a:pPr>
             <a:r>
-              <a:rPr sz="1300"/>
+              <a:rPr b="1" sz="1300"/>
               <a:t>Milwaukee Airport Аномалии на температурите за целият период</a:t>
             </a:r>
           </a:p>
@@ -1181,11 +1182,11 @@
           </c:val>
         </c:ser>
         <c:marker val="0"/>
-        <c:axId val="52249837"/>
-        <c:axId val="69142401"/>
+        <c:axId val="33848154"/>
+        <c:axId val="73083942"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="52249837"/>
+        <c:axId val="33848154"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1201,14 +1202,14 @@
             </a:solidFill>
           </a:ln>
         </c:spPr>
-        <c:crossAx val="69142401"/>
+        <c:crossAx val="73083942"/>
         <c:crossesAt val="0"/>
         <c:lblAlgn val="ctr"/>
         <c:auto val="1"/>
         <c:lblOffset val="100"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="69142401"/>
+        <c:axId val="73083942"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1233,7 +1234,7 @@
             </a:solidFill>
           </a:ln>
         </c:spPr>
-        <c:crossAx val="52249837"/>
+        <c:crossAx val="33848154"/>
         <c:crossesAt val="0"/>
       </c:valAx>
       <c:spPr>
@@ -1261,7 +1262,7 @@
 </c:chartSpace>
 </file>
 
-<file path=xl/charts/chart391.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/charts/chart111.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:lang val="en-US"/>
   <c:chart>
@@ -1276,7 +1277,7 @@
               <a:defRPr/>
             </a:pPr>
             <a:r>
-              <a:rPr sz="1300"/>
+              <a:rPr b="1" sz="1300"/>
               <a:t>Milwaukee Airport Сезонни температури за целят период</a:t>
             </a:r>
           </a:p>
@@ -2480,11 +2481,11 @@
           </c:val>
         </c:ser>
         <c:marker val="0"/>
-        <c:axId val="56945936"/>
-        <c:axId val="89704074"/>
+        <c:axId val="92506109"/>
+        <c:axId val="91005918"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="56945936"/>
+        <c:axId val="92506109"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2500,14 +2501,14 @@
             </a:solidFill>
           </a:ln>
         </c:spPr>
-        <c:crossAx val="89704074"/>
+        <c:crossAx val="91005918"/>
         <c:crossesAt val="0"/>
         <c:lblAlgn val="ctr"/>
         <c:auto val="1"/>
         <c:lblOffset val="100"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="89704074"/>
+        <c:axId val="91005918"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2532,7 +2533,7 @@
             </a:solidFill>
           </a:ln>
         </c:spPr>
-        <c:crossAx val="56945936"/>
+        <c:crossAx val="92506109"/>
         <c:crossesAt val="0"/>
       </c:valAx>
       <c:spPr>
@@ -2560,7 +2561,7 @@
 </c:chartSpace>
 </file>
 
-<file path=xl/charts/chart392.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/charts/chart112.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:lang val="en-US"/>
   <c:chart>
@@ -2575,7 +2576,7 @@
               <a:defRPr/>
             </a:pPr>
             <a:r>
-              <a:rPr sz="1300"/>
+              <a:rPr b="1" sz="1300"/>
               <a:t>Milwaukee Airport Средни сезонни температури за 2та периода</a:t>
             </a:r>
           </a:p>
@@ -2727,11 +2728,11 @@
           </c:val>
         </c:ser>
         <c:marker val="0"/>
-        <c:axId val="19909606"/>
-        <c:axId val="50396022"/>
+        <c:axId val="44236116"/>
+        <c:axId val="96686100"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="19909606"/>
+        <c:axId val="44236116"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2747,14 +2748,14 @@
             </a:solidFill>
           </a:ln>
         </c:spPr>
-        <c:crossAx val="50396022"/>
+        <c:crossAx val="96686100"/>
         <c:crossesAt val="0"/>
         <c:lblAlgn val="ctr"/>
         <c:auto val="1"/>
         <c:lblOffset val="100"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="50396022"/>
+        <c:axId val="96686100"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2779,7 +2780,7 @@
             </a:solidFill>
           </a:ln>
         </c:spPr>
-        <c:crossAx val="19909606"/>
+        <c:crossAx val="44236116"/>
         <c:crossesAt val="0"/>
       </c:valAx>
       <c:spPr>
@@ -2807,7 +2808,7 @@
 </c:chartSpace>
 </file>
 
-<file path=xl/charts/chart393.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/charts/chart113.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:lang val="en-US"/>
   <c:chart>
@@ -2822,8 +2823,8 @@
               <a:defRPr/>
             </a:pPr>
             <a:r>
-              <a:rPr sz="1300"/>
-              <a:t>Milwaukee Airport Средни месечни температури за 2та периода</a:t>
+              <a:rPr b="1" sz="1300"/>
+              <a:t>Milwaukee Airport Средни месечни валежи за 2та периода</a:t>
             </a:r>
           </a:p>
         </c:rich>
@@ -3053,11 +3054,11 @@
           </c:val>
         </c:ser>
         <c:gapWidth val="100"/>
-        <c:axId val="68798334"/>
-        <c:axId val="26022314"/>
+        <c:axId val="54422708"/>
+        <c:axId val="40714415"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="68798334"/>
+        <c:axId val="54422708"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3073,14 +3074,14 @@
             </a:solidFill>
           </a:ln>
         </c:spPr>
-        <c:crossAx val="26022314"/>
+        <c:crossAx val="40714415"/>
         <c:crossesAt val="0"/>
         <c:lblAlgn val="ctr"/>
         <c:auto val="1"/>
         <c:lblOffset val="100"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="26022314"/>
+        <c:axId val="40714415"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3105,7 +3106,7 @@
             </a:solidFill>
           </a:ln>
         </c:spPr>
-        <c:crossAx val="68798334"/>
+        <c:crossAx val="54422708"/>
         <c:crossesAt val="0"/>
       </c:valAx>
       <c:spPr>
@@ -3133,7 +3134,7 @@
 </c:chartSpace>
 </file>
 
-<file path=xl/charts/chart394.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/charts/chart114.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:lang val="en-US"/>
   <c:chart>
@@ -3148,7 +3149,7 @@
               <a:defRPr/>
             </a:pPr>
             <a:r>
-              <a:rPr sz="1300"/>
+              <a:rPr b="1" sz="1300"/>
               <a:t>Milwaukee Airport Аномалии на валежите за целият период</a:t>
             </a:r>
           </a:p>
@@ -3450,11 +3451,11 @@
           </c:val>
         </c:ser>
         <c:gapWidth val="100"/>
-        <c:axId val="46330419"/>
-        <c:axId val="74037559"/>
+        <c:axId val="45217097"/>
+        <c:axId val="25245503"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="46330419"/>
+        <c:axId val="45217097"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3470,14 +3471,14 @@
             </a:solidFill>
           </a:ln>
         </c:spPr>
-        <c:crossAx val="74037559"/>
+        <c:crossAx val="25245503"/>
         <c:crossesAt val="0"/>
         <c:lblAlgn val="ctr"/>
         <c:auto val="1"/>
         <c:lblOffset val="100"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="74037559"/>
+        <c:axId val="25245503"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3502,7 +3503,7 @@
             </a:solidFill>
           </a:ln>
         </c:spPr>
-        <c:crossAx val="46330419"/>
+        <c:crossAx val="45217097"/>
         <c:crossesAt val="0"/>
       </c:valAx>
       <c:spPr>
@@ -3530,7 +3531,7 @@
 </c:chartSpace>
 </file>
 
-<file path=xl/charts/chart395.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/charts/chart115.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:lang val="en-US"/>
   <c:chart>
@@ -3545,7 +3546,7 @@
               <a:defRPr/>
             </a:pPr>
             <a:r>
-              <a:rPr sz="1300"/>
+              <a:rPr b="1" sz="1300"/>
               <a:t>Milwaukee Airport Сезонни валежи за целят период</a:t>
             </a:r>
           </a:p>
@@ -4749,11 +4750,11 @@
           </c:val>
         </c:ser>
         <c:marker val="0"/>
-        <c:axId val="81992712"/>
-        <c:axId val="47943389"/>
+        <c:axId val="18841601"/>
+        <c:axId val="90204137"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="81992712"/>
+        <c:axId val="18841601"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -4769,14 +4770,14 @@
             </a:solidFill>
           </a:ln>
         </c:spPr>
-        <c:crossAx val="47943389"/>
+        <c:crossAx val="90204137"/>
         <c:crossesAt val="0"/>
         <c:lblAlgn val="ctr"/>
         <c:auto val="1"/>
         <c:lblOffset val="100"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="47943389"/>
+        <c:axId val="90204137"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -4801,7 +4802,7 @@
             </a:solidFill>
           </a:ln>
         </c:spPr>
-        <c:crossAx val="81992712"/>
+        <c:crossAx val="18841601"/>
         <c:crossesAt val="0"/>
       </c:valAx>
       <c:spPr>
@@ -4829,7 +4830,7 @@
 </c:chartSpace>
 </file>
 
-<file path=xl/charts/chart396.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/charts/chart116.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:lang val="en-US"/>
   <c:chart>
@@ -4844,7 +4845,7 @@
               <a:defRPr/>
             </a:pPr>
             <a:r>
-              <a:rPr sz="1300"/>
+              <a:rPr b="1" sz="1300"/>
               <a:t>Milwaukee Airport Средни сезонни валежи за 2та периода</a:t>
             </a:r>
           </a:p>
@@ -4996,11 +4997,11 @@
           </c:val>
         </c:ser>
         <c:marker val="0"/>
-        <c:axId val="87353269"/>
-        <c:axId val="30843880"/>
+        <c:axId val="82613738"/>
+        <c:axId val="20154491"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="87353269"/>
+        <c:axId val="82613738"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -5016,14 +5017,14 @@
             </a:solidFill>
           </a:ln>
         </c:spPr>
-        <c:crossAx val="30843880"/>
+        <c:crossAx val="20154491"/>
         <c:crossesAt val="0"/>
         <c:lblAlgn val="ctr"/>
         <c:auto val="1"/>
         <c:lblOffset val="100"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="30843880"/>
+        <c:axId val="20154491"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -5048,7 +5049,7 @@
             </a:solidFill>
           </a:ln>
         </c:spPr>
-        <c:crossAx val="87353269"/>
+        <c:crossAx val="82613738"/>
         <c:crossesAt val="0"/>
       </c:valAx>
       <c:spPr>
@@ -5076,7 +5077,7 @@
 </c:chartSpace>
 </file>
 
-<file path=xl/charts/chart397.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/charts/chart117.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:lang val="en-US"/>
   <c:chart>
@@ -5091,7 +5092,7 @@
               <a:defRPr/>
             </a:pPr>
             <a:r>
-              <a:rPr sz="1300"/>
+              <a:rPr b="1" sz="1300"/>
               <a:t>Milwaukee Airport Средни сезонни валежи за 2та периода</a:t>
             </a:r>
           </a:p>
@@ -5226,11 +5227,11 @@
           </c:val>
         </c:ser>
         <c:gapWidth val="100"/>
-        <c:axId val="69526181"/>
-        <c:axId val="80053122"/>
+        <c:axId val="95526709"/>
+        <c:axId val="47756202"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="69526181"/>
+        <c:axId val="95526709"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -5246,14 +5247,14 @@
             </a:solidFill>
           </a:ln>
         </c:spPr>
-        <c:crossAx val="80053122"/>
+        <c:crossAx val="47756202"/>
         <c:crossesAt val="0"/>
         <c:lblAlgn val="ctr"/>
         <c:auto val="1"/>
         <c:lblOffset val="100"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="80053122"/>
+        <c:axId val="47756202"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -5278,7 +5279,7 @@
             </a:solidFill>
           </a:ln>
         </c:spPr>
-        <c:crossAx val="69526181"/>
+        <c:crossAx val="95526709"/>
         <c:crossesAt val="0"/>
       </c:valAx>
       <c:spPr>
@@ -5311,15 +5312,15 @@
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
       <xdr:col>0</xdr:col>
-      <xdr:colOff>330480</xdr:colOff>
+      <xdr:colOff>357480</xdr:colOff>
       <xdr:row>68</xdr:row>
-      <xdr:rowOff>162000</xdr:rowOff>
+      <xdr:rowOff>153000</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>22</xdr:col>
-      <xdr:colOff>236160</xdr:colOff>
+      <xdr:colOff>262800</xdr:colOff>
       <xdr:row>88</xdr:row>
-      <xdr:rowOff>23400</xdr:rowOff>
+      <xdr:rowOff>14040</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame>
       <xdr:nvGraphicFramePr>
@@ -5327,8 +5328,8 @@
         <xdr:cNvGraphicFramePr/>
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
-        <a:off x="330480" y="11647800"/>
-        <a:ext cx="9697320" cy="3239640"/>
+        <a:off x="357480" y="11638800"/>
+        <a:ext cx="9795240" cy="3239280"/>
       </xdr:xfrm>
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
@@ -5341,15 +5342,15 @@
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
       <xdr:col>0</xdr:col>
-      <xdr:colOff>192960</xdr:colOff>
+      <xdr:colOff>219960</xdr:colOff>
       <xdr:row>44</xdr:row>
-      <xdr:rowOff>164520</xdr:rowOff>
+      <xdr:rowOff>155520</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>22</xdr:col>
-      <xdr:colOff>226080</xdr:colOff>
+      <xdr:colOff>252720</xdr:colOff>
       <xdr:row>64</xdr:row>
-      <xdr:rowOff>25920</xdr:rowOff>
+      <xdr:rowOff>16560</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame>
       <xdr:nvGraphicFramePr>
@@ -5357,8 +5358,8 @@
         <xdr:cNvGraphicFramePr/>
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
-        <a:off x="192960" y="7596360"/>
-        <a:ext cx="9824760" cy="3239640"/>
+        <a:off x="219960" y="7587360"/>
+        <a:ext cx="9922680" cy="3239280"/>
       </xdr:xfrm>
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
@@ -5371,15 +5372,15 @@
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
       <xdr:col>23</xdr:col>
-      <xdr:colOff>649440</xdr:colOff>
+      <xdr:colOff>676440</xdr:colOff>
       <xdr:row>1</xdr:row>
-      <xdr:rowOff>155160</xdr:rowOff>
+      <xdr:rowOff>146160</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>35</xdr:col>
-      <xdr:colOff>15840</xdr:colOff>
+      <xdr:colOff>42480</xdr:colOff>
       <xdr:row>21</xdr:row>
-      <xdr:rowOff>16560</xdr:rowOff>
+      <xdr:rowOff>7200</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame>
       <xdr:nvGraphicFramePr>
@@ -5387,8 +5388,8 @@
         <xdr:cNvGraphicFramePr/>
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
-        <a:off x="10814400" y="324000"/>
-        <a:ext cx="7443000" cy="3239640"/>
+        <a:off x="10943640" y="315000"/>
+        <a:ext cx="7523280" cy="3239280"/>
       </xdr:xfrm>
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
@@ -5401,15 +5402,15 @@
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
       <xdr:col>23</xdr:col>
-      <xdr:colOff>646560</xdr:colOff>
-      <xdr:row>29</xdr:row>
-      <xdr:rowOff>6840</xdr:rowOff>
+      <xdr:colOff>673560</xdr:colOff>
+      <xdr:row>28</xdr:row>
+      <xdr:rowOff>166680</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>32</xdr:col>
-      <xdr:colOff>768240</xdr:colOff>
+      <xdr:colOff>794880</xdr:colOff>
       <xdr:row>48</xdr:row>
-      <xdr:rowOff>37080</xdr:rowOff>
+      <xdr:rowOff>27720</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame>
       <xdr:nvGraphicFramePr>
@@ -5417,8 +5418,8 @@
         <xdr:cNvGraphicFramePr/>
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
-        <a:off x="10811520" y="4905000"/>
-        <a:ext cx="5759640" cy="3239640"/>
+        <a:off x="10940760" y="4896000"/>
+        <a:ext cx="5815440" cy="3239280"/>
       </xdr:xfrm>
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
@@ -5436,15 +5437,15 @@
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
       <xdr:col>0</xdr:col>
-      <xdr:colOff>330480</xdr:colOff>
+      <xdr:colOff>357480</xdr:colOff>
       <xdr:row>68</xdr:row>
-      <xdr:rowOff>162000</xdr:rowOff>
+      <xdr:rowOff>153000</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>22</xdr:col>
-      <xdr:colOff>63720</xdr:colOff>
+      <xdr:colOff>90360</xdr:colOff>
       <xdr:row>88</xdr:row>
-      <xdr:rowOff>23400</xdr:rowOff>
+      <xdr:rowOff>14040</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame>
       <xdr:nvGraphicFramePr>
@@ -5452,8 +5453,8 @@
         <xdr:cNvGraphicFramePr/>
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
-        <a:off x="330480" y="11647800"/>
-        <a:ext cx="9697320" cy="3239640"/>
+        <a:off x="357480" y="11638800"/>
+        <a:ext cx="9797400" cy="3239280"/>
       </xdr:xfrm>
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
@@ -5466,15 +5467,15 @@
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
       <xdr:col>0</xdr:col>
-      <xdr:colOff>192960</xdr:colOff>
+      <xdr:colOff>219960</xdr:colOff>
       <xdr:row>44</xdr:row>
-      <xdr:rowOff>164520</xdr:rowOff>
+      <xdr:rowOff>155520</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>22</xdr:col>
-      <xdr:colOff>53640</xdr:colOff>
+      <xdr:colOff>80280</xdr:colOff>
       <xdr:row>64</xdr:row>
-      <xdr:rowOff>25920</xdr:rowOff>
+      <xdr:rowOff>16560</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame>
       <xdr:nvGraphicFramePr>
@@ -5482,8 +5483,8 @@
         <xdr:cNvGraphicFramePr/>
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
-        <a:off x="192960" y="7596360"/>
-        <a:ext cx="9824760" cy="3239640"/>
+        <a:off x="219960" y="7587360"/>
+        <a:ext cx="9924840" cy="3239280"/>
       </xdr:xfrm>
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
@@ -5496,15 +5497,15 @@
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
       <xdr:col>23</xdr:col>
-      <xdr:colOff>476640</xdr:colOff>
+      <xdr:colOff>503640</xdr:colOff>
       <xdr:row>1</xdr:row>
-      <xdr:rowOff>155160</xdr:rowOff>
+      <xdr:rowOff>146160</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>34</xdr:col>
-      <xdr:colOff>655920</xdr:colOff>
+      <xdr:colOff>682560</xdr:colOff>
       <xdr:row>21</xdr:row>
-      <xdr:rowOff>16560</xdr:rowOff>
+      <xdr:rowOff>7200</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame>
       <xdr:nvGraphicFramePr>
@@ -5512,8 +5513,8 @@
         <xdr:cNvGraphicFramePr/>
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
-        <a:off x="10814400" y="324000"/>
-        <a:ext cx="7443000" cy="3239640"/>
+        <a:off x="10945440" y="315000"/>
+        <a:ext cx="7515000" cy="3239280"/>
       </xdr:xfrm>
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
@@ -5525,16 +5526,16 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
-      <xdr:col>23</xdr:col>
-      <xdr:colOff>804960</xdr:colOff>
+      <xdr:col>24</xdr:col>
+      <xdr:colOff>10800</xdr:colOff>
       <xdr:row>28</xdr:row>
-      <xdr:rowOff>145800</xdr:rowOff>
+      <xdr:rowOff>136800</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>33</xdr:col>
-      <xdr:colOff>113760</xdr:colOff>
-      <xdr:row>48</xdr:row>
-      <xdr:rowOff>7200</xdr:rowOff>
+      <xdr:colOff>140400</xdr:colOff>
+      <xdr:row>47</xdr:row>
+      <xdr:rowOff>166680</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame>
       <xdr:nvGraphicFramePr>
@@ -5542,8 +5543,8 @@
         <xdr:cNvGraphicFramePr/>
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
-        <a:off x="11142720" y="4875120"/>
-        <a:ext cx="5759640" cy="3239640"/>
+        <a:off x="11273760" y="4866120"/>
+        <a:ext cx="5823360" cy="3239280"/>
       </xdr:xfrm>
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
@@ -5556,15 +5557,15 @@
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
       <xdr:col>24</xdr:col>
-      <xdr:colOff>9000</xdr:colOff>
-      <xdr:row>50</xdr:row>
-      <xdr:rowOff>720</xdr:rowOff>
+      <xdr:colOff>36000</xdr:colOff>
+      <xdr:row>49</xdr:row>
+      <xdr:rowOff>160560</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>33</xdr:col>
-      <xdr:colOff>130320</xdr:colOff>
+      <xdr:colOff>156960</xdr:colOff>
       <xdr:row>69</xdr:row>
-      <xdr:rowOff>30960</xdr:rowOff>
+      <xdr:rowOff>21600</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame>
       <xdr:nvGraphicFramePr>
@@ -5572,8 +5573,8 @@
         <xdr:cNvGraphicFramePr/>
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
-        <a:off x="11159280" y="8445960"/>
-        <a:ext cx="5759640" cy="3239640"/>
+        <a:off x="11298960" y="8436960"/>
+        <a:ext cx="5814720" cy="3239280"/>
       </xdr:xfrm>
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
@@ -5599,19 +5600,18 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="7.90816326530612"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="6.99489795918367"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="6.86734693877551"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="5.93877551020408"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="10.4132653061225"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="6.86734693877551"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="6.45408163265306"/>
-    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="5.53571428571429"/>
-    <col collapsed="false" hidden="false" max="9" min="9" style="0" width="5.41836734693878"/>
-    <col collapsed="false" hidden="false" max="10" min="10" style="0" width="6.45408163265306"/>
-    <col collapsed="false" hidden="false" max="11" min="11" style="0" width="5.65816326530612"/>
-    <col collapsed="false" hidden="false" max="12" min="12" style="0" width="5.79591836734694"/>
-    <col collapsed="false" hidden="false" max="1025" min="13" style="0" width="8.8469387755102"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="7.98979591836735"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="7.06632653061225"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="6.93877551020408"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="6.00510204081633"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="10.5204081632653"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="6.93877551020408"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="6.52551020408163"/>
+    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="5.58673469387755"/>
+    <col collapsed="false" hidden="false" max="9" min="9" style="0" width="5.46938775510204"/>
+    <col collapsed="false" hidden="false" max="10" min="10" style="0" width="6.52551020408163"/>
+    <col collapsed="false" hidden="false" max="11" min="11" style="0" width="5.71428571428571"/>
+    <col collapsed="false" hidden="false" max="12" min="12" style="0" width="5.85714285714286"/>
   </cols>
   <sheetData>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.3" outlineLevel="0" r="1">
@@ -7388,33 +7388,33 @@
   </sheetPr>
   <dimension ref="A1:AC68"/>
   <sheetViews>
-    <sheetView colorId="64" defaultGridColor="true" rightToLeft="false" showFormulas="false" showGridLines="true" showOutlineSymbols="true" showRowColHeaders="true" showZeros="true" tabSelected="false" topLeftCell="A1" view="normal" windowProtection="false" workbookViewId="0" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100">
-      <selection activeCell="Y58" activeCellId="0" pane="topLeft" sqref="Y58"/>
+    <sheetView colorId="64" defaultGridColor="true" rightToLeft="false" showFormulas="false" showGridLines="true" showOutlineSymbols="true" showRowColHeaders="true" showZeros="true" tabSelected="false" topLeftCell="A25" view="normal" windowProtection="false" workbookViewId="0" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100">
+      <selection activeCell="AE50" activeCellId="0" pane="topLeft" sqref="AE50"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.3"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="6.45408163265306"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="6.19897959183674"/>
-    <col collapsed="false" hidden="false" max="4" min="3" style="0" width="5.29081632653061"/>
-    <col collapsed="false" hidden="false" max="9" min="5" style="0" width="5.55102040816327"/>
-    <col collapsed="false" hidden="false" max="10" min="10" style="0" width="5.81122448979592"/>
-    <col collapsed="false" hidden="false" max="11" min="11" style="0" width="5.55102040816327"/>
-    <col collapsed="false" hidden="false" max="13" min="12" style="0" width="5.29081632653061"/>
-    <col collapsed="false" hidden="false" max="14" min="14" style="0" width="5.55102040816327"/>
-    <col collapsed="false" hidden="false" max="16" min="15" style="0" width="9.16326530612245"/>
-    <col collapsed="false" hidden="false" max="17" min="17" style="0" width="8.64795918367347"/>
-    <col collapsed="false" hidden="false" max="18" min="18" style="0" width="9.16326530612245"/>
-    <col collapsed="false" hidden="false" max="19" min="19" style="0" width="6.45408163265306"/>
-    <col collapsed="false" hidden="false" max="20" min="20" style="0" width="6.3265306122449"/>
-    <col collapsed="false" hidden="false" max="22" min="21" style="0" width="5.67857142857143"/>
-    <col collapsed="false" hidden="false" max="23" min="23" style="0" width="5.29081632653061"/>
-    <col collapsed="false" hidden="false" max="24" min="24" style="0" width="11.5204081632653"/>
-    <col collapsed="false" hidden="false" max="25" min="25" style="0" width="11.2295918367347"/>
-    <col collapsed="false" hidden="false" max="26" min="26" style="0" width="6.3265306122449"/>
-    <col collapsed="false" hidden="false" max="28" min="27" style="0" width="5.55102040816327"/>
-    <col collapsed="false" hidden="false" max="29" min="29" style="0" width="5.16326530612245"/>
-    <col collapsed="false" hidden="false" max="1025" min="30" style="0" width="11.5204081632653"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="6.52551020408163"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="6.26530612244898"/>
+    <col collapsed="false" hidden="false" max="4" min="3" style="0" width="5.3469387755102"/>
+    <col collapsed="false" hidden="false" max="9" min="5" style="0" width="5.60714285714286"/>
+    <col collapsed="false" hidden="false" max="10" min="10" style="0" width="5.87755102040816"/>
+    <col collapsed="false" hidden="false" max="11" min="11" style="0" width="5.60714285714286"/>
+    <col collapsed="false" hidden="false" max="13" min="12" style="0" width="5.3469387755102"/>
+    <col collapsed="false" hidden="false" max="14" min="14" style="0" width="5.60714285714286"/>
+    <col collapsed="false" hidden="false" max="16" min="15" style="0" width="9.25"/>
+    <col collapsed="false" hidden="false" max="17" min="17" style="0" width="8.73979591836735"/>
+    <col collapsed="false" hidden="false" max="18" min="18" style="0" width="9.25"/>
+    <col collapsed="false" hidden="false" max="19" min="19" style="0" width="6.52551020408163"/>
+    <col collapsed="false" hidden="false" max="20" min="20" style="0" width="6.38775510204082"/>
+    <col collapsed="false" hidden="false" max="22" min="21" style="0" width="5.73469387755102"/>
+    <col collapsed="false" hidden="false" max="23" min="23" style="0" width="5.3469387755102"/>
+    <col collapsed="false" hidden="false" max="24" min="24" style="0" width="11.6377551020408"/>
+    <col collapsed="false" hidden="false" max="25" min="25" style="0" width="11.3418367346939"/>
+    <col collapsed="false" hidden="false" max="26" min="26" style="0" width="6.38775510204082"/>
+    <col collapsed="false" hidden="false" max="28" min="27" style="0" width="5.60714285714286"/>
+    <col collapsed="false" hidden="false" max="29" min="29" style="0" width="5.20918367346939"/>
+    <col collapsed="false" hidden="false" max="1025" min="30" style="0" width="11.6377551020408"/>
   </cols>
   <sheetData>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.3" outlineLevel="0" r="1">
@@ -10694,33 +10694,33 @@
   </sheetPr>
   <dimension ref="A1:AC68"/>
   <sheetViews>
-    <sheetView colorId="64" defaultGridColor="true" rightToLeft="false" showFormulas="false" showGridLines="true" showOutlineSymbols="true" showRowColHeaders="true" showZeros="true" tabSelected="true" topLeftCell="A13" view="normal" windowProtection="false" workbookViewId="0" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100">
-      <selection activeCell="M33" activeCellId="0" pane="topLeft" sqref="M33"/>
+    <sheetView colorId="64" defaultGridColor="true" rightToLeft="false" showFormulas="false" showGridLines="true" showOutlineSymbols="true" showRowColHeaders="true" showZeros="true" tabSelected="true" topLeftCell="P31" view="normal" windowProtection="false" workbookViewId="0" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100">
+      <selection activeCell="X45" activeCellId="0" pane="topLeft" sqref="X45"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.3"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="6.45408163265306"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="6.19897959183674"/>
-    <col collapsed="false" hidden="false" max="4" min="3" style="0" width="5.29081632653061"/>
-    <col collapsed="false" hidden="false" max="9" min="5" style="0" width="5.55102040816327"/>
-    <col collapsed="false" hidden="false" max="10" min="10" style="0" width="5.81122448979592"/>
-    <col collapsed="false" hidden="false" max="11" min="11" style="0" width="5.55102040816327"/>
-    <col collapsed="false" hidden="false" max="13" min="12" style="0" width="5.29081632653061"/>
-    <col collapsed="false" hidden="false" max="14" min="14" style="0" width="8"/>
-    <col collapsed="false" hidden="false" max="16" min="15" style="0" width="9.16326530612245"/>
-    <col collapsed="false" hidden="false" max="17" min="17" style="0" width="8.64795918367347"/>
-    <col collapsed="false" hidden="false" max="18" min="18" style="0" width="9.16326530612245"/>
-    <col collapsed="false" hidden="false" max="19" min="19" style="0" width="6.45408163265306"/>
-    <col collapsed="false" hidden="false" max="20" min="20" style="0" width="6.3265306122449"/>
-    <col collapsed="false" hidden="false" max="22" min="21" style="0" width="5.67857142857143"/>
-    <col collapsed="false" hidden="false" max="23" min="23" style="0" width="5.29081632653061"/>
-    <col collapsed="false" hidden="false" max="24" min="24" style="0" width="11.5204081632653"/>
-    <col collapsed="false" hidden="false" max="25" min="25" style="0" width="11.2295918367347"/>
-    <col collapsed="false" hidden="false" max="26" min="26" style="0" width="6.3265306122449"/>
-    <col collapsed="false" hidden="false" max="28" min="27" style="0" width="5.55102040816327"/>
-    <col collapsed="false" hidden="false" max="29" min="29" style="0" width="5.16326530612245"/>
-    <col collapsed="false" hidden="false" max="1025" min="30" style="0" width="11.5204081632653"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="6.52551020408163"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="6.26530612244898"/>
+    <col collapsed="false" hidden="false" max="4" min="3" style="0" width="5.3469387755102"/>
+    <col collapsed="false" hidden="false" max="9" min="5" style="0" width="5.60714285714286"/>
+    <col collapsed="false" hidden="false" max="10" min="10" style="0" width="5.87755102040816"/>
+    <col collapsed="false" hidden="false" max="11" min="11" style="0" width="5.60714285714286"/>
+    <col collapsed="false" hidden="false" max="13" min="12" style="0" width="5.3469387755102"/>
+    <col collapsed="false" hidden="false" max="14" min="14" style="0" width="8.08163265306122"/>
+    <col collapsed="false" hidden="false" max="16" min="15" style="0" width="9.25"/>
+    <col collapsed="false" hidden="false" max="17" min="17" style="0" width="8.73979591836735"/>
+    <col collapsed="false" hidden="false" max="18" min="18" style="0" width="9.25"/>
+    <col collapsed="false" hidden="false" max="19" min="19" style="0" width="6.52551020408163"/>
+    <col collapsed="false" hidden="false" max="20" min="20" style="0" width="6.38775510204082"/>
+    <col collapsed="false" hidden="false" max="22" min="21" style="0" width="5.73469387755102"/>
+    <col collapsed="false" hidden="false" max="23" min="23" style="0" width="5.3469387755102"/>
+    <col collapsed="false" hidden="false" max="24" min="24" style="0" width="11.6377551020408"/>
+    <col collapsed="false" hidden="false" max="25" min="25" style="0" width="11.3418367346939"/>
+    <col collapsed="false" hidden="false" max="26" min="26" style="0" width="6.38775510204082"/>
+    <col collapsed="false" hidden="false" max="28" min="27" style="0" width="5.60714285714286"/>
+    <col collapsed="false" hidden="false" max="29" min="29" style="0" width="5.20918367346939"/>
+    <col collapsed="false" hidden="false" max="1025" min="30" style="0" width="11.6377551020408"/>
   </cols>
   <sheetData>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.3" outlineLevel="0" r="1">

</xml_diff>